<commit_message>
Confidence regions for experiments
Experiment 2
Experiment 3
</commit_message>
<xml_diff>
--- a/Coding/Save results.xlsx
+++ b/Coding/Save results.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment 1" sheetId="1" r:id="rId1"/>
     <sheet name="Experiment 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Experiment 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="21">
   <si>
     <t>Y</t>
   </si>
@@ -85,6 +86,9 @@
   </si>
   <si>
     <t>boys2</t>
+  </si>
+  <si>
+    <t>girls2</t>
   </si>
 </sst>
 </file>
@@ -925,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12:K27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,4 +1374,471 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>52474</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>15030</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>38678</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>13959</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>70211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>20027</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>32345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>11930</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <f>SUM(E2,E4,E6,E8)</f>
+        <v>193708</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8">
+        <f>E2</f>
+        <v>52474</v>
+      </c>
+      <c r="C12" s="7">
+        <f>B12/$B$11</f>
+        <v>0.27089227084064676</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8">
+        <f>E4</f>
+        <v>38678</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" ref="C13:C15" si="0">B13/$B$11</f>
+        <v>0.19967167076217812</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8">
+        <f>E6</f>
+        <v>70211</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.3624579263633923</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="8">
+        <f>E8</f>
+        <v>32345</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>0.16697813203378281</v>
+      </c>
+      <c r="N15" s="1"/>
+      <c r="S15" s="3"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="7"/>
+      <c r="N16" s="6"/>
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="8">
+        <f>E3+E5+E7+E9</f>
+        <v>60946</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="N17" s="1"/>
+      <c r="S17" s="3"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="8">
+        <f>E3</f>
+        <v>15030</v>
+      </c>
+      <c r="C18" s="7">
+        <f>B18/$B$17</f>
+        <v>0.24661175466806681</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="8">
+        <f>E5</f>
+        <v>13959</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" ref="C19:C21" si="1">B19/$B$17</f>
+        <v>0.22903882125159977</v>
+      </c>
+      <c r="N19" s="1"/>
+      <c r="S19" s="3"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="8">
+        <f>E7</f>
+        <v>20027</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="1"/>
+        <v>0.32860236931053721</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="8">
+        <f>E9</f>
+        <v>11930</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="1"/>
+        <v>0.1957470547697962</v>
+      </c>
+      <c r="N21" s="1"/>
+      <c r="S21" s="3"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="N22" s="6"/>
+      <c r="S22" s="2"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="N23" s="1"/>
+      <c r="S23" s="3"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="7">
+        <f>MAX(C14+C15,C20+C21)</f>
+        <v>0.52943605839717511</v>
+      </c>
+      <c r="C24" s="7">
+        <f>MIN(C13+C14+C15,C19+C20+C21)</f>
+        <v>0.72910772915935329</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24">
+        <v>0.52689520000000001</v>
+      </c>
+      <c r="G24">
+        <v>0.73107279999999997</v>
+      </c>
+      <c r="N24" s="6"/>
+      <c r="S24" s="2"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="7">
+        <f>MAX(C15,C21)</f>
+        <v>0.1957470547697962</v>
+      </c>
+      <c r="C25" s="7">
+        <f>MIN(C15+C14,C21+C20)</f>
+        <v>0.52434942408033347</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25">
+        <v>0.1927372</v>
+      </c>
+      <c r="G25">
+        <v>0.52887930000000005</v>
+      </c>
+      <c r="N25" s="1"/>
+      <c r="S25" s="3"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="N26" s="6"/>
+      <c r="S26" s="2"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="N27" s="1"/>
+      <c r="S27" s="3"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="7">
+        <f>MAX(C14,C20)</f>
+        <v>0.3624579263633923</v>
+      </c>
+      <c r="C28" s="7">
+        <f>MIN(C14+C15,C20+C21)</f>
+        <v>0.52434942408033347</v>
+      </c>
+      <c r="E28" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28">
+        <v>0.3603287</v>
+      </c>
+      <c r="G28">
+        <v>0.52887930000000005</v>
+      </c>
+      <c r="N28" s="6"/>
+      <c r="S28" s="2"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="7">
+        <f>MAX(C15+C14,C21+C20)</f>
+        <v>0.52943605839717511</v>
+      </c>
+      <c r="C29" s="7">
+        <f>MIN(C12+C14+C15,C18+C20+C21)</f>
+        <v>0.77096117874840031</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29">
+        <v>0.52689520000000001</v>
+      </c>
+      <c r="G29">
+        <v>0.77417729999999996</v>
+      </c>
+      <c r="N29" s="1"/>
+      <c r="S29" s="3"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S30" s="4"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S31" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Calculated ATE for instruments
Just need to run confidence regions for final three experiments and
instruments are done
</commit_message>
<xml_diff>
--- a/Coding/Save results.xlsx
+++ b/Coding/Save results.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\econ-fs\Home3\zctpep9\GitHub\Covariatesets\Coding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11985" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment 1" sheetId="1" r:id="rId1"/>
@@ -17,8 +12,11 @@
     <sheet name="Experiment 3" sheetId="3" r:id="rId3"/>
     <sheet name="Experiment 4" sheetId="4" r:id="rId4"/>
     <sheet name="Experiment 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Experiment 6" sheetId="6" r:id="rId6"/>
+    <sheet name="Experiment 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Experiment 8" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="36">
   <si>
     <t>Y</t>
   </si>
@@ -122,15 +120,30 @@
   <si>
     <t>Z=girlboy</t>
   </si>
+  <si>
+    <t>multi2nd</t>
+  </si>
+  <si>
+    <t>samesex</t>
+  </si>
+  <si>
+    <t>Z=2</t>
+  </si>
+  <si>
+    <t>boy2</t>
+  </si>
+  <si>
+    <t>girl2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +162,22 @@
       <color rgb="FF0000FF"/>
       <name val="Lucida Console"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -191,8 +220,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +497,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,7 +508,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="A23" sqref="A23:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2546,7 +2578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
@@ -3533,4 +3565,2547 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>67504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>51528</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>90238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>43266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="8"/>
+      <c r="C10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <f>SUM(E2:E3,E5:E6)</f>
+        <v>252536</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="8">
+        <f>E2</f>
+        <v>67504</v>
+      </c>
+      <c r="C12" s="7">
+        <f>B12/$B$11</f>
+        <v>0.26730446352203252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="8">
+        <f>E3</f>
+        <v>51528</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" ref="C13:C15" si="0">B13/$B$11</f>
+        <v>0.20404219596413978</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="8">
+        <f>E5</f>
+        <v>90238</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.35732727215129723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="8">
+        <f>E6</f>
+        <v>43266</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="0"/>
+        <v>0.1713260683625305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="8"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="8">
+        <f>SUM(E4,E7)</f>
+        <v>2118</v>
+      </c>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="8">
+        <v>0</v>
+      </c>
+      <c r="C18" s="7">
+        <f>B18/$B$17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="8">
+        <f>E4</f>
+        <v>1109</v>
+      </c>
+      <c r="C19" s="7">
+        <f t="shared" ref="C19:C21" si="1">B19/$B$17</f>
+        <v>0.52360717658168088</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="8">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="8">
+        <f>E7</f>
+        <v>1009</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" si="1"/>
+        <v>0.47639282341831918</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="7">
+        <f>MAX(C14+C15,C20+C21)</f>
+        <v>0.52865334051382773</v>
+      </c>
+      <c r="C24" s="7">
+        <f>MIN(C13+C14+C15,C19+C20+C21)</f>
+        <v>0.73269553647796748</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="7">
+        <f>MAX(C15,C21)</f>
+        <v>0.47639282341831918</v>
+      </c>
+      <c r="C25" s="7">
+        <f>MIN(C15+C14,C21+C20)</f>
+        <v>0.47639282341831918</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="10">
+        <f>MAX(C14,C20)</f>
+        <v>0.35732727215129723</v>
+      </c>
+      <c r="C28" s="10">
+        <f>MIN(C14+C15,C20+C21)</f>
+        <v>0.47639282341831918</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="10">
+        <f>MAX(C15+C14,C21+C20)</f>
+        <v>0.52865334051382773</v>
+      </c>
+      <c r="C29" s="10">
+        <f>MIN(C12+C14+C15,C18+C20+C21)</f>
+        <v>0.47639282341831918</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>35186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>32318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>23066</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>28462</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>47105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>43133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>19519</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>23747</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <f>SUM(F2,F4,F8,F10)</f>
+        <v>124876</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="8">
+        <f>F2</f>
+        <v>35186</v>
+      </c>
+      <c r="C16" s="7">
+        <f>B16/$B$15</f>
+        <v>0.28176751337326628</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="7">
+        <f>MAX(C18+C19,C24+C25,C30+C31)</f>
+        <v>0.53352125308305842</v>
+      </c>
+      <c r="G16" s="7">
+        <f>1-MAX(C16,C22,C28)</f>
+        <v>0.71823248662673378</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="8">
+        <f>F4</f>
+        <v>23066</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" ref="C17:C18" si="0">B17/$B$15</f>
+        <v>0.18471123354367533</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="7">
+        <f>MAX(C19,C25,C31)</f>
+        <v>0.47639282341831918</v>
+      </c>
+      <c r="G17" s="7">
+        <f>MIN(C18+C19,C24+C25,C30+C31)</f>
+        <v>0.47639282341831918</v>
+      </c>
+      <c r="I17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="8">
+        <f>F8</f>
+        <v>47105</v>
+      </c>
+      <c r="C18" s="7">
+        <f t="shared" si="0"/>
+        <v>0.37721419648291105</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="8">
+        <f>F10</f>
+        <v>19519</v>
+      </c>
+      <c r="C19" s="7">
+        <f>B19/$B$15</f>
+        <v>0.15630705660014735</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="7"/>
+      <c r="E20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="10">
+        <f>MAX(C18,C24,C30)</f>
+        <v>0.37721419648291105</v>
+      </c>
+      <c r="G20" s="10">
+        <f>MIN(C19+C18,C24+C25,C31+C30)</f>
+        <v>0.47639282341831918</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="8">
+        <f>SUM(F6,F7,F12,F13)</f>
+        <v>2118</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="E21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="10">
+        <f>MAX(C19+C18,C24+C25,C31+C30)</f>
+        <v>0.53352125308305842</v>
+      </c>
+      <c r="G21" s="10">
+        <f>1-MAX(C17,C23,C29)</f>
+        <v>0.47639282341831912</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="8">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="C22" s="7">
+        <f>B22/$B$21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="8">
+        <f>SUM(F6:F7)</f>
+        <v>1109</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" ref="C23:C25" si="1">B23/$B$21</f>
+        <v>0.52360717658168088</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="8">
+        <f>SUM(F12:F13)</f>
+        <v>1009</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" si="1"/>
+        <v>0.47639282341831918</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="7"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="8">
+        <f>SUM(F3,F5,F9,F11)</f>
+        <v>127660</v>
+      </c>
+      <c r="C27" s="7"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="8">
+        <f>F3</f>
+        <v>32318</v>
+      </c>
+      <c r="C28" s="7">
+        <f>B28/$B$27</f>
+        <v>0.25315682281059065</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="8">
+        <f>F5</f>
+        <v>28462</v>
+      </c>
+      <c r="C29" s="7">
+        <f t="shared" ref="C29:C31" si="2">B29/$B$27</f>
+        <v>0.22295159016136612</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="8">
+        <f>F9</f>
+        <v>43133</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" si="2"/>
+        <v>0.33787404041986524</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="8">
+        <f>F11</f>
+        <v>23747</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" si="2"/>
+        <v>0.18601754660817799</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>15030</v>
+      </c>
+      <c r="K2">
+        <f>D2</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>(1-D2)*G2*(1-H2)</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>(1-D2)*(1-G2)*H2</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>(1-D2)*G2*H2</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f>(1-D2)*(1-G2)*(1-H2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>13716</v>
+      </c>
+      <c r="K3">
+        <f>D3</f>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f>(1-D3)*G3*(1-H3)</f>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f>(1-D3)*(1-G3)*H3</f>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f>(1-D3)*G3*H3</f>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f>(1-D3)*(1-G3)*(1-H3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>20027</v>
+      </c>
+      <c r="K4">
+        <f>D4</f>
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <f>(1-D4)*G4*(1-H4)</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f>(1-D4)*(1-G4)*H4</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f>(1-D4)*G4*H4</f>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>(1-D4)*(1-G4)*(1-H4)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>11673</v>
+      </c>
+      <c r="K5">
+        <f>D5</f>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f>(1-D5)*G5*(1-H5)</f>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <f>(1-D5)*(1-G5)*H5</f>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f>(1-D5)*G5*H5</f>
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <f>(1-D5)*(1-G5)*(1-H5)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>17288</v>
+      </c>
+      <c r="K6">
+        <f>D6</f>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f>(1-D6)*G6*(1-H6)</f>
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <f>(1-D6)*(1-G6)*H6</f>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f>(1-D6)*G6*H6</f>
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <f>(1-D6)*(1-G6)*(1-H6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>14746</v>
+      </c>
+      <c r="K7">
+        <f>D7</f>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f>(1-D7)*G7*(1-H7)</f>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f>(1-D7)*(1-G7)*H7</f>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f>(1-D7)*G7*H7</f>
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f>(1-D7)*(1-G7)*(1-H7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>23106</v>
+      </c>
+      <c r="K8">
+        <f>D8</f>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f>(1-D8)*G8*(1-H8)</f>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f>(1-D8)*(1-G8)*H8</f>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f>(1-D8)*G8*H8</f>
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <f>(1-D8)*(1-G8)*(1-H8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>12074</v>
+      </c>
+      <c r="K9">
+        <f>D9</f>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f>(1-D9)*G9*(1-H9)</f>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <f>(1-D9)*(1-G9)*H9</f>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f>(1-D9)*G9*H9</f>
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <f>(1-D9)*(1-G9)*(1-H9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>17664</v>
+      </c>
+      <c r="K10">
+        <f>D10</f>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f>(1-D10)*G10*(1-H10)</f>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <f>(1-D10)*(1-G10)*H10</f>
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <f>(1-D10)*G10*H10</f>
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>(1-D10)*(1-G10)*(1-H10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>11565</v>
+      </c>
+      <c r="K11">
+        <f>D11</f>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f>(1-D11)*G11*(1-H11)</f>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f>(1-D11)*(1-G11)*H11</f>
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <f>(1-D11)*G11*H11</f>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>(1-D11)*(1-G11)*(1-H11)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>23323</v>
+      </c>
+      <c r="K12">
+        <f>D12</f>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f>(1-D12)*G12*(1-H12)</f>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f>(1-D12)*(1-G12)*H12</f>
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <f>(1-D12)*G12*H12</f>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>(1-D12)*(1-G12)*(1-H12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>9653</v>
+      </c>
+      <c r="K13">
+        <f>D13</f>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f>(1-D13)*G13*(1-H13)</f>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f>(1-D13)*(1-G13)*H13</f>
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <f>(1-D13)*G13*H13</f>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>(1-D13)*(1-G13)*(1-H13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>17522</v>
+      </c>
+      <c r="K14">
+        <f>D14</f>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f>(1-D14)*G14*(1-H14)</f>
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <f>(1-D14)*(1-G14)*H14</f>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f>(1-D14)*G14*H14</f>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>(1-D14)*(1-G14)*(1-H14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>11501</v>
+      </c>
+      <c r="K15">
+        <f>D15</f>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f>(1-D15)*G15*(1-H15)</f>
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <f>(1-D15)*(1-G15)*H15</f>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f>(1-D15)*G15*H15</f>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>(1-D15)*(1-G15)*(1-H15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>23782</v>
+      </c>
+      <c r="K16">
+        <f>D16</f>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>(1-D16)*G16*(1-H16)</f>
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <f>(1-D16)*(1-G16)*H16</f>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <f>(1-D16)*G16*H16</f>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>(1-D16)*(1-G16)*(1-H16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>9866</v>
+      </c>
+      <c r="K17">
+        <f>D17</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>(1-D17)*G17*(1-H17)</f>
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <f>(1-D17)*(1-G17)*H17</f>
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <f>(1-D17)*G17*H17</f>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>(1-D17)*(1-G17)*(1-H17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>275</v>
+      </c>
+      <c r="K18">
+        <f>D18</f>
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <f>(1-D18)*G18*(1-H18)</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f>(1-D18)*(1-G18)*H18</f>
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <f>(1-D18)*G18*H18</f>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>(1-D18)*(1-G18)*(1-H18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>283</v>
+      </c>
+      <c r="K19">
+        <f>D19</f>
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <f>(1-D19)*G19*(1-H19)</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f>(1-D19)*(1-G19)*H19</f>
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <f>(1-D19)*G19*H19</f>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f>(1-D19)*(1-G19)*(1-H19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>243</v>
+      </c>
+      <c r="K20">
+        <f>D20</f>
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f>(1-D20)*G20*(1-H20)</f>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f>(1-D20)*(1-G20)*H20</f>
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <f>(1-D20)*G20*H20</f>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>(1-D20)*(1-G20)*(1-H20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>308</v>
+      </c>
+      <c r="K21">
+        <f>D21</f>
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <f>(1-D21)*G21*(1-H21)</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>(1-D21)*(1-G21)*H21</f>
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <f>(1-D21)*G21*H21</f>
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>(1-D21)*(1-G21)*(1-H21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>244</v>
+      </c>
+      <c r="K22">
+        <f>D22</f>
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <f>(1-D22)*G22*(1-H22)</f>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f>(1-D22)*(1-G22)*H22</f>
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <f>(1-D22)*G22*H22</f>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>(1-D22)*(1-G22)*(1-H22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>231</v>
+      </c>
+      <c r="K23">
+        <f>D23</f>
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <f>(1-D23)*G23*(1-H23)</f>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>(1-D23)*(1-G23)*H23</f>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f>(1-D23)*G23*H23</f>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>(1-D23)*(1-G23)*(1-H23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>257</v>
+      </c>
+      <c r="K24">
+        <f>D24</f>
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <f>(1-D24)*G24*(1-H24)</f>
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f>(1-D24)*(1-G24)*H24</f>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f>(1-D24)*G24*H24</f>
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f>(1-D24)*(1-G24)*(1-H24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>277</v>
+      </c>
+      <c r="K25">
+        <f>D25</f>
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <f>(1-D25)*G25*(1-H25)</f>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f>(1-D25)*(1-G25)*H25</f>
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <f>(1-D25)*G25*H25</f>
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f>(1-D25)*(1-G25)*(1-H25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>5</v>
+      </c>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" t="s">
+        <v>11</v>
+      </c>
+      <c r="N27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f>I2</f>
+        <v>15030</v>
+      </c>
+      <c r="D28">
+        <f>I6</f>
+        <v>17288</v>
+      </c>
+      <c r="E28">
+        <f>I10</f>
+        <v>17664</v>
+      </c>
+      <c r="F28">
+        <f>I14</f>
+        <v>17522</v>
+      </c>
+      <c r="H28" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="7">
+        <f>MAX(B36+B35,C35+C36,D35+D36,E35+E36,F35+F36)</f>
+        <v>0.53689904421502765</v>
+      </c>
+      <c r="J28" s="7">
+        <f>1-MAX(B33:F33)</f>
+        <v>0.71603568844948162</v>
+      </c>
+      <c r="L28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <f>SUM(I18:I21)</f>
+        <v>1109</v>
+      </c>
+      <c r="C29">
+        <f t="shared" ref="C29:C31" si="0">I3</f>
+        <v>13716</v>
+      </c>
+      <c r="D29">
+        <f t="shared" ref="D29:D31" si="1">I7</f>
+        <v>14746</v>
+      </c>
+      <c r="E29">
+        <f t="shared" ref="E29:E31" si="2">I11</f>
+        <v>11565</v>
+      </c>
+      <c r="F29">
+        <f t="shared" ref="F29:F31" si="3">I15</f>
+        <v>11501</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="7">
+        <f>MAX(B36:F36)</f>
+        <v>0.47639282341831918</v>
+      </c>
+      <c r="J29" s="7">
+        <f>MIN(B36+B35,C35+C36,D35+D36,E35+E36,F35+F36)</f>
+        <v>0.47639282341831918</v>
+      </c>
+      <c r="L29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>20027</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>23106</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>23323</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="3"/>
+        <v>23782</v>
+      </c>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <f>SUM(I22:I25)</f>
+        <v>1009</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>11673</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>12074</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>9653</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="3"/>
+        <v>9866</v>
+      </c>
+      <c r="H31" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N31" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="11">
+        <f>SUM(B28:B31)</f>
+        <v>2118</v>
+      </c>
+      <c r="C32" s="11">
+        <f t="shared" ref="C32:F32" si="4">SUM(C28:C31)</f>
+        <v>60446</v>
+      </c>
+      <c r="D32" s="11">
+        <f t="shared" si="4"/>
+        <v>67214</v>
+      </c>
+      <c r="E32" s="11">
+        <f t="shared" si="4"/>
+        <v>62205</v>
+      </c>
+      <c r="F32" s="11">
+        <f t="shared" si="4"/>
+        <v>62671</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="10">
+        <f>MAX(J18,J24)</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="10">
+        <f>MIN(J18+J19,J24+J25)</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M32" s="9">
+        <v>0.37147950000000002</v>
+      </c>
+      <c r="N32" s="9">
+        <v>0.52674080000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <f>B28/B$32</f>
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:F33" si="5">C28/C$32</f>
+        <v>0.24865168911094199</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="5"/>
+        <v>0.25720831969530156</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="5"/>
+        <v>0.28396431155051843</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="5"/>
+        <v>0.27958704983166055</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="10">
+        <f>MAX(J19+J18,J25+J24)</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="10">
+        <f>MIN(J16+J18+J19,J22+J24+J25)</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M33" s="9">
+        <v>0.52976509999999999</v>
+      </c>
+      <c r="N33" s="9">
+        <v>0.77685899999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ref="B34:F34" si="6">B29/B$32</f>
+        <v>0.52360717658168088</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="6"/>
+        <v>0.22691327796711114</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="6"/>
+        <v>0.21938881780581426</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="6"/>
+        <v>0.18591753074511697</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="6"/>
+        <v>0.18351390595331174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ref="B35:F35" si="7">B30/B$32</f>
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="7"/>
+        <v>0.33132051748668234</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="7"/>
+        <v>0.34376766745023357</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="7"/>
+        <v>0.37493770597218873</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="7"/>
+        <v>0.3794737597932058</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36">
+        <f t="shared" ref="B36:F36" si="8">B31/B$32</f>
+        <v>0.47639282341831918</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="8"/>
+        <v>0.19311451543526453</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="8"/>
+        <v>0.17963519504865058</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="8"/>
+        <v>0.15518045173217587</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="8"/>
+        <v>0.15742528442182188</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:O25">
+    <sortCondition ref="K2:K25"/>
+    <sortCondition ref="L2:L25"/>
+    <sortCondition ref="M2:M25"/>
+    <sortCondition ref="N2:N25"/>
+    <sortCondition ref="O2:O25"/>
+    <sortCondition ref="B2:B25"/>
+    <sortCondition ref="C2:C25"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>